<commit_message>
added separate report and screenshot code
</commit_message>
<xml_diff>
--- a/jbkowp/src/test/resources/OwpTestData.xlsx
+++ b/jbkowp/src/test/resources/OwpTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14520" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15360" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Username</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>123</t>
-  </si>
-  <si>
-    <t>123456</t>
   </si>
 </sst>
 </file>
@@ -443,7 +440,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -511,9 +508,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Add dashboardpage and user
</commit_message>
<xml_diff>
--- a/jbkowp/src/test/resources/OwpTestData.xlsx
+++ b/jbkowp/src/test/resources/OwpTestData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15075" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13500" windowHeight="6330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Registration" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:L19"/>
+  <oleSize ref="A1:M19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -69,6 +70,27 @@
   </si>
   <si>
     <t>123456</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>eamil</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>subhash</t>
+  </si>
+  <si>
+    <t>9876545677</t>
+  </si>
+  <si>
+    <t>User registered successfully.</t>
   </si>
 </sst>
 </file>
@@ -442,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -524,4 +546,75 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update TEST NG Version
</commit_message>
<xml_diff>
--- a/jbkowp/src/test/resources/OwpTestData.xlsx
+++ b/jbkowp/src/test/resources/OwpTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15360" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13590" windowHeight="6330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="AddUser" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:F19"/>
+  <oleSize ref="A1:K19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Username</t>
   </si>
@@ -92,12 +92,54 @@
   </si>
   <si>
     <t>MAIN NAVIGATION</t>
+  </si>
+  <si>
+    <t>tcid</t>
+  </si>
+  <si>
+    <t>tcinfo</t>
+  </si>
+  <si>
+    <t>selectvalue</t>
+  </si>
+  <si>
+    <t>selenium</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Cources</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>8654852352</t>
+  </si>
+  <si>
+    <t>ingale.subhash@gmail.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>validInfo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -157,12 +199,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -465,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -555,7 +599,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -623,14 +667,88 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A2" s="1">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>